<commit_message>
reviewed and OK'd mapping respiration
</commit_message>
<xml_diff>
--- a/Mappings/Respiration - STU3.xlsx
+++ b/Mappings/Respiration - STU3.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3671155D-FCC7-49BB-82BF-0F47CB8B7452}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="260">
   <si>
     <t>Subject</t>
   </si>
@@ -760,12 +754,6 @@
     <t>.administeredOxygen (extension)</t>
   </si>
   <si>
-    <t>.administeredOxygen.flowrate</t>
-  </si>
-  <si>
-    <t>.administeredOxyge.fiO2</t>
-  </si>
-  <si>
     <t>.administeredOxygen.administrationDevice (extensions MedicalDevice)</t>
   </si>
   <si>
@@ -806,12 +794,21 @@
   </si>
   <si>
     <t>Constraint that this may only be present if extraOxygenAdministration is present and true</t>
+  </si>
+  <si>
+    <t>.administeredOxygen.fiO2</t>
+  </si>
+  <si>
+    <t>.administeredOxygen.flowRate</t>
+  </si>
+  <si>
+    <t>part of the HCIM medicaldevice.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1039,16 +1036,16 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Ongeldig 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ongeldig 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1274,7 +1271,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1315,7 +1312,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1356,7 +1353,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1411,14 +1408,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10241"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1426,29 +1420,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1478,14 +1449,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10242"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1493,29 +1461,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1545,14 +1490,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10243"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1560,29 +1502,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1612,14 +1531,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10244"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1627,29 +1543,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1679,14 +1572,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10245"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1694,29 +1584,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1746,14 +1613,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10246"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1761,29 +1625,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1813,14 +1654,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10247"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1828,29 +1666,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1880,14 +1695,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10248"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1895,29 +1707,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1947,14 +1736,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10249"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1962,29 +1748,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2014,14 +1777,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10250"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2029,29 +1789,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2081,14 +1818,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10251"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2096,29 +1830,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2148,14 +1859,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10252"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2163,29 +1871,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2215,14 +1900,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10253"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2230,29 +1912,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2282,14 +1941,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10254"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2297,29 +1953,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2349,14 +1982,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10255"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2364,29 +1994,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2416,14 +2023,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10256"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2431,29 +2035,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2483,14 +2064,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10257"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2498,29 +2076,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2550,14 +2105,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10258"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2565,29 +2117,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2617,14 +2146,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10259"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2632,29 +2158,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2684,14 +2187,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10260"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2699,29 +2199,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2751,14 +2228,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10261"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000015280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2766,29 +2240,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2818,14 +2269,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10262"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2833,29 +2281,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2885,14 +2310,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10263"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000017280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2900,29 +2322,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2952,14 +2351,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10264"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000018280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2967,29 +2363,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3019,14 +2392,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10265"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000019280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3034,29 +2404,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3086,14 +2433,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10266"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3101,29 +2445,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3153,14 +2474,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10267"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3168,29 +2486,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3220,14 +2515,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10268"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3235,29 +2527,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3287,14 +2556,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10269"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3302,29 +2568,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3354,14 +2597,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10270"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3369,29 +2609,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3421,14 +2638,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10271"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001F280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3436,29 +2650,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3488,14 +2679,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10272"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000020280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3503,29 +2691,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3555,14 +2720,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10273"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000021280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3570,29 +2732,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3622,14 +2761,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10274"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000022280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3637,29 +2773,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3689,14 +2802,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10275"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000023280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3704,29 +2814,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3756,14 +2843,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10276"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000024280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3771,29 +2855,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3823,14 +2884,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10277"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000025280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3838,29 +2896,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3890,14 +2925,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10278"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000026280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3905,29 +2937,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3957,14 +2966,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10279"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000027280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -3972,29 +2978,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4024,14 +3007,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10280"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000028280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4039,29 +3019,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4091,14 +3048,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10281"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000029280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4106,29 +3060,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4158,14 +3089,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10282"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002A280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4173,29 +3101,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4225,14 +3130,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10283"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002B280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4240,29 +3142,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4292,14 +3171,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10284"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002C280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4307,29 +3183,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4359,14 +3212,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10285"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002D280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4374,29 +3224,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4426,14 +3253,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10286"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002E280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4441,29 +3265,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4493,14 +3294,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10287"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002F280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4508,29 +3306,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4560,14 +3335,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10288"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000030280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4575,29 +3347,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4627,14 +3376,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s10289"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000031280000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -4642,29 +3388,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4964,14 +3687,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5080,7 +3803,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -5091,7 +3814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5137,7 +3860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5149,10 +3872,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -5344,7 +4067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5361,7 +4084,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43ADBDF4-FEEB-41F1-A4E6-F9778249E32F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6721,11 +5444,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6826,7 +5549,7 @@
       </c>
       <c r="R3" s="23"/>
       <c r="S3" s="27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="T3" s="23" t="s">
         <v>241</v>
@@ -6865,12 +5588,12 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
       <c r="T4" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
@@ -6904,7 +5627,7 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
@@ -6945,16 +5668,16 @@
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="S6" s="22" t="s">
         <v>2</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
@@ -6992,16 +5715,16 @@
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="S7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
@@ -7039,16 +5762,16 @@
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="R8" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="S8" s="22" t="s">
         <v>2</v>
       </c>
       <c r="T8" s="22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="2:20" ht="51" x14ac:dyDescent="0.2">
@@ -7082,12 +5805,12 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
-      <c r="T9" s="29" t="s">
-        <v>257</v>
+      <c r="T9" s="28" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
@@ -7163,7 +5886,7 @@
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="2:20" ht="51" x14ac:dyDescent="0.2">
@@ -7198,8 +5921,8 @@
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
-      <c r="Q12" s="22" t="s">
-        <v>243</v>
+      <c r="Q12" s="28" t="s">
+        <v>258</v>
       </c>
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
@@ -7237,8 +5960,8 @@
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
-      <c r="Q13" s="22" t="s">
-        <v>244</v>
+      <c r="Q13" s="28" t="s">
+        <v>257</v>
       </c>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
@@ -7275,7 +5998,7 @@
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
@@ -7311,20 +6034,22 @@
         <v>142</v>
       </c>
       <c r="P15" s="2"/>
-      <c r="Q15" s="22" t="s">
-        <v>246</v>
+      <c r="Q15" s="28" t="s">
+        <v>244</v>
       </c>
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
+      <c r="T15" s="28" t="s">
+        <v>259</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O6" location="RhythmCodelist!A1" display="RhythmCodelist" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="O7" location="DepthCodelist!A1" display="DepthCodelist" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="O8" location="DeviatingBreathingPatternCodeli!A1" display="DeviatingBreathingPatternCodelist" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="O14" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="O15" location="AdministrationDeviceCodelist!A1" display="AdministrationDeviceCodelist" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="O6" location="RhythmCodelist!A1" display="RhythmCodelist"/>
+    <hyperlink ref="O7" location="DepthCodelist!A1" display="DepthCodelist"/>
+    <hyperlink ref="O8" location="DeviatingBreathingPatternCodeli!A1" display="DeviatingBreathingPatternCodelist"/>
+    <hyperlink ref="O14" r:id="rId1"/>
+    <hyperlink ref="O15" location="AdministrationDeviceCodelist!A1" display="AdministrationDeviceCodelist"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -7335,7 +6060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7350,15 +6075,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
@@ -7458,7 +6183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7473,15 +6198,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
@@ -7581,7 +6306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7596,15 +6321,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
@@ -7789,7 +6514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7804,15 +6529,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">

</xml_diff>